<commit_message>
None error catch issues
Having some issues with trying to catch this error
</commit_message>
<xml_diff>
--- a/converted_data.xlsx
+++ b/converted_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,33 +448,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>first build</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>'Test Prop 1'</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Horace's Home</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2016-12-19</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2017-01-23</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
going back to basics
getting my for loop to accurately put basic data into the cells that is needed.

too many variables to deal with causing issues.

stripping it down to the basics. Now i can update this to write my data
</commit_message>
<xml_diff>
--- a/converted_data.xlsx
+++ b/converted_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,27 +424,135 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Task</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Set Part</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Parent Build</t>
+          <t>C</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Start Date</t>
+          <t>D</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>End Date</t>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>E</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
going back to sorting section
going back to simplify and fix issues with sorting and make it more straightforward to work better for my code later on
</commit_message>
<xml_diff>
--- a/converted_data.xlsx
+++ b/converted_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,141 +448,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Working data to cells
Data goes to the correct cells now!
</commit_message>
<xml_diff>
--- a/converted_data.xlsx
+++ b/converted_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,6 +448,276 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>design</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Test Prop 1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2016-12-05</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2016-12-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>design</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Test Prop 2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2016-12-13</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2016-12-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>first build</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Test Prop 1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2016-12-19</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2017-01-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>first build</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Test Prop 2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2016-12-23</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2017-01-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>design</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Test Prop 2</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2017-01-09</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2017-01-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>first build</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Test Prop 3</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2017-01-23</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2017-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>first build</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Test Prop 4</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2017-01-23</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2017-02-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>first build</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Test Prop 5</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2017-01-26</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2017-02-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>duplicate build</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Test Prop 1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Horace's Home</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2017-03-20</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2017-03-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>duplicate build</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Test Prop 2</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Horace's Home 2</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2017-03-20</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2017-03-24</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>